<commit_message>
added order number to invoice
</commit_message>
<xml_diff>
--- a/src/Server/InvoiceTemplate.xlsx
+++ b/src/Server/InvoiceTemplate.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SpinGee\repos\TaxManager\src\Server\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F528EA63-B04E-42BA-AFEC-8A4CABD94BBF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D093A4AD-4D35-40C9-B77D-AF5D1A22C1BD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="405" yWindow="1230" windowWidth="15330" windowHeight="10890" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -121,9 +121,6 @@
     <t>Sazba MD: 6000Kč</t>
   </si>
   <si>
-    <t>Číslo obj.: 17Zak00002</t>
-  </si>
-  <si>
     <t>Datum uskutečnění zdanit. Plnění</t>
   </si>
   <si>
@@ -149,6 +146,9 @@
   </si>
   <si>
     <t>:3.9.2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Číslo obj.: </t>
   </si>
 </sst>
 </file>
@@ -786,17 +786,14 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -824,12 +821,15 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20 % – Zvýraznění 1" xfId="1" builtinId="30" customBuiltin="1"/>
@@ -1238,8 +1238,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10:D10"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1252,14 +1252,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="46" t="s">
+      <c r="B1" s="30"/>
+      <c r="C1" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="46"/>
+      <c r="D1" s="31"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
@@ -1272,7 +1272,7 @@
         <v>3</v>
       </c>
       <c r="D2" s="21" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -1296,30 +1296,30 @@
       <c r="D4" s="5"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="34" t="s">
+      <c r="A5" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="34"/>
+      <c r="B5" s="29"/>
       <c r="C5" s="4" t="s">
         <v>7</v>
       </c>
       <c r="D5" s="22" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="34" t="s">
+      <c r="A6" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="34"/>
+      <c r="B6" s="29"/>
       <c r="C6" s="4"/>
       <c r="D6" s="6"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="34" t="s">
+      <c r="A7" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="34"/>
+      <c r="B7" s="29"/>
       <c r="C7" s="2" t="s">
         <v>8</v>
       </c>
@@ -1328,8 +1328,8 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="34"/>
-      <c r="B8" s="34"/>
+      <c r="A8" s="29"/>
+      <c r="B8" s="29"/>
       <c r="C8" s="4" t="s">
         <v>9</v>
       </c>
@@ -1338,8 +1338,8 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="34"/>
-      <c r="B9" s="34"/>
+      <c r="A9" s="29"/>
+      <c r="B9" s="29"/>
       <c r="C9" s="4"/>
       <c r="D9" s="5"/>
     </row>
@@ -1350,8 +1350,8 @@
       <c r="B10" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="35"/>
-      <c r="D10" s="36"/>
+      <c r="C10" s="32"/>
+      <c r="D10" s="33"/>
       <c r="G10" s="28"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
@@ -1361,71 +1361,71 @@
       <c r="B11" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="29"/>
-      <c r="D11" s="30"/>
+      <c r="C11" s="42"/>
+      <c r="D11" s="43"/>
       <c r="G11" s="28"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="4"/>
       <c r="B12" s="5"/>
-      <c r="C12" s="29"/>
-      <c r="D12" s="30"/>
+      <c r="C12" s="42"/>
+      <c r="D12" s="43"/>
     </row>
     <row r="13" spans="1:7" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4"/>
       <c r="B13" s="8"/>
-      <c r="C13" s="41"/>
-      <c r="D13" s="42"/>
+      <c r="C13" s="38"/>
+      <c r="D13" s="39"/>
     </row>
     <row r="14" spans="1:7" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="10"/>
       <c r="B14" s="11"/>
-      <c r="C14" s="43"/>
-      <c r="D14" s="44"/>
+      <c r="C14" s="40"/>
+      <c r="D14" s="41"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" s="37" t="s">
-        <v>33</v>
-      </c>
-      <c r="B15" s="38"/>
+      <c r="A15" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" s="35"/>
       <c r="C15" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="D15" s="12"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" s="44" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" s="44"/>
+      <c r="C16" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="D15" s="12"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" s="31" t="s">
-        <v>12</v>
-      </c>
-      <c r="B16" s="31"/>
-      <c r="C16" s="23" t="s">
-        <v>41</v>
-      </c>
       <c r="D16" s="5"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="31" t="s">
+      <c r="A17" s="44" t="s">
         <v>13</v>
       </c>
-      <c r="B17" s="31"/>
+      <c r="B17" s="44"/>
       <c r="C17" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D17" s="5"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="32" t="s">
+      <c r="A18" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="B18" s="32"/>
+      <c r="B18" s="45"/>
       <c r="C18" s="24" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D18" s="11"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="25" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D20" s="13"/>
     </row>
@@ -1437,10 +1437,10 @@
     </row>
     <row r="23" spans="1:4" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="25" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B23" s="25" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
@@ -1453,22 +1453,22 @@
     </row>
     <row r="25" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A25" s="16"/>
-      <c r="B25" s="40" t="s">
+      <c r="B25" s="37" t="s">
         <v>28</v>
       </c>
-      <c r="C25" s="40"/>
+      <c r="C25" s="37"/>
       <c r="D25" s="26" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="16"/>
-      <c r="B26" s="39" t="s">
+      <c r="B26" s="36" t="s">
         <v>29</v>
       </c>
-      <c r="C26" s="39"/>
+      <c r="C26" s="36"/>
       <c r="D26" s="26" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -1477,7 +1477,7 @@
         <v>16</v>
       </c>
       <c r="D27" s="19" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
@@ -1490,12 +1490,12 @@
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A47" s="33" t="s">
+      <c r="A47" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="B47" s="33"/>
-      <c r="C47" s="33"/>
-      <c r="D47" s="33"/>
+      <c r="B47" s="46"/>
+      <c r="C47" s="46"/>
+      <c r="D47" s="46"/>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
@@ -1518,12 +1518,7 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A47:D47"/>
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="C10:D10"/>
     <mergeCell ref="A15:B15"/>
@@ -1534,7 +1529,12 @@
     <mergeCell ref="A16:B16"/>
     <mergeCell ref="A17:B17"/>
     <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A47:D47"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
   </mergeCells>
   <pageMargins left="0.74791666666666667" right="0.74791666666666667" top="0.98402777777777783" bottom="0.98402777777777783" header="0.51180555555555562" footer="0.51180555555555562"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>